<commit_message>
Documents: Fitxers de shape i de la bd
</commit_message>
<xml_diff>
--- a/documents/BaseMaps.xlsx
+++ b/documents/BaseMaps.xlsx
@@ -142,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +161,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -195,11 +209,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -498,7 +514,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -646,16 +662,16 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -730,13 +746,14 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>